<commit_message>
Gonzalo: escenarios de riesgo prelim
</commit_message>
<xml_diff>
--- a/Riesgo/DataTarea_Exogenas_Riesgo6.xlsx
+++ b/Riesgo/DataTarea_Exogenas_Riesgo6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\CUECOPolMon\Riesgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EFEFE5-C799-4767-9890-DF6A909ABDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE60F2A3-8013-48A1-8D38-01F55F69FFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="2655" windowWidth="21540" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="2310" windowWidth="21540" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uvar" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
         <v>45747</v>
       </c>
       <c r="B3" s="4">
-        <v>-0.20513363517789199</v>
+        <v>-0.10513400000000001</v>
       </c>
       <c r="C3" s="4">
         <v>5.5</v>
@@ -586,7 +586,7 @@
         <v>45838</v>
       </c>
       <c r="B4" s="4">
-        <v>-0.121548563572178</v>
+        <v>7.8451000000000007E-2</v>
       </c>
       <c r="C4" s="4">
         <v>5.5</v>
@@ -604,7 +604,7 @@
         <v>45930</v>
       </c>
       <c r="B5" s="4">
-        <v>-3.8264805610782202E-2</v>
+        <v>0.21173500000000001</v>
       </c>
       <c r="C5" s="4">
         <v>5.5</v>
@@ -622,7 +622,7 @@
         <v>46022</v>
       </c>
       <c r="B6" s="4">
-        <v>0.02</v>
+        <v>0.27</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
@@ -640,7 +640,7 @@
         <v>46112</v>
       </c>
       <c r="B7" s="4">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -658,7 +658,7 @@
         <v>46203</v>
       </c>
       <c r="B8" s="4">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="C8" s="4">
         <v>2.5</v>
@@ -676,7 +676,7 @@
         <v>46295</v>
       </c>
       <c r="B9" s="4">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="C9" s="4">
         <v>2.5</v>
@@ -694,7 +694,7 @@
         <v>46387</v>
       </c>
       <c r="B10" s="4">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="C10" s="4">
         <v>2.5</v>

</xml_diff>